<commit_message>
perbaikan bug sesuai revisi hasil sosialiasi siak V1.2 dengan akademik
</commit_message>
<xml_diff>
--- a/public/assets/report_classroom/Classroom_loan_report_1.xlsx
+++ b/public/assets/report_classroom/Classroom_loan_report_1.xlsx
@@ -16,12 +16,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="48">
   <si>
     <t>DATA PEMINJAMAN RUANG KELAS UNTUK KEGIATAN NON AKADEMIK</t>
   </si>
   <si>
-    <t>Tahun Ajar 23/24 Semester 2</t>
+    <t>TAHUN AJAR 23/24 SEMESTER 2</t>
   </si>
   <si>
     <t>NO</t>
@@ -69,7 +69,52 @@
     <t>TANGGAL APROVAL ADMIN</t>
   </si>
   <si>
-    <t>DATA PEMINJAMAN RUANG KELAS TIDAK TERSEDIA</t>
+    <t>pleno</t>
+  </si>
+  <si>
+    <t>RKA.KJ.01.001</t>
+  </si>
+  <si>
+    <t>KAMPUS A DAAN MOGOT</t>
+  </si>
+  <si>
+    <t>02/07/2024</t>
+  </si>
+  <si>
+    <t>06:30 - 08:30</t>
+  </si>
+  <si>
+    <t>MEGA LESTARI</t>
+  </si>
+  <si>
+    <t>organization</t>
+  </si>
+  <si>
+    <t>PMK</t>
+  </si>
+  <si>
+    <t>SANTO GUNAWAN</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>HIZKIA ANJU PASARIBU</t>
+  </si>
+  <si>
+    <t>01/07/2024 - 09:46</t>
+  </si>
+  <si>
+    <t>ujian</t>
+  </si>
+  <si>
+    <t>05/07/2024</t>
+  </si>
+  <si>
+    <t>other</t>
+  </si>
+  <si>
+    <t>27/06/2024 - 10:04</t>
   </si>
   <si>
     <t>DATA PEMINJAMAN RUANG KELAS UNTUK KEGIATAN AKADEMIK ( KELAS PENGGANTI )</t>
@@ -90,22 +135,16 @@
     <t>ALASAN MENGGANTI KELAS</t>
   </si>
   <si>
-    <t>RKA.KJ.01.001</t>
-  </si>
-  <si>
-    <t>KAMPUS A DAAN MOGOT</t>
-  </si>
-  <si>
-    <t>11/06/2024</t>
-  </si>
-  <si>
-    <t>06:30 - 08:30</t>
+    <t>03/07/2024</t>
+  </si>
+  <si>
+    <t>13:30 - 15:30</t>
   </si>
   <si>
     <t>DEMI ADIDRANA</t>
   </si>
   <si>
-    <t>07/06/2024 12:30</t>
+    <t>21/06/2024 12:30</t>
   </si>
   <si>
     <t>matematika</t>
@@ -114,34 +153,13 @@
     <t>d3tt-kj-21-0001</t>
   </si>
   <si>
-    <t>S1 Teknologi Informasi</t>
-  </si>
-  <si>
-    <t>ga tau</t>
-  </si>
-  <si>
-    <t>10/06/2024 - 14:29</t>
-  </si>
-  <si>
-    <t>22/06/2024</t>
-  </si>
-  <si>
-    <t>08:30 - 09:30</t>
-  </si>
-  <si>
-    <t>ALVA NURVINA SULARSO</t>
-  </si>
-  <si>
-    <t>Pengajuan Penetration Testing untuk sistem peminjaman asset unit logistik (Silo)</t>
-  </si>
-  <si>
-    <t>D3TT-KJ-21-001</t>
+    <t>S1 Sistem Informasi</t>
   </si>
   <si>
     <t>sakit</t>
   </si>
   <si>
-    <t>13/06/2024 - 11:15</t>
+    <t>27/06/2024 - 10:16</t>
   </si>
 </sst>
 </file>
@@ -219,7 +237,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0"/>
     <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="1">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
@@ -231,13 +249,10 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
     <xf xfId="0" fontId="1" numFmtId="0" fillId="0" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0"/>
-    <xf xfId="0" fontId="1" numFmtId="0" fillId="0" borderId="1" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
+    <xf xfId="0" fontId="1" numFmtId="0" fillId="0" borderId="1" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="0"/>
     <xf xfId="0" fontId="2" numFmtId="0" fillId="2" borderId="1" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
     </xf>
-    <xf xfId="0" fontId="1" numFmtId="0" fillId="0" borderId="1" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -537,7 +552,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:O6"/>
+  <dimension ref="A1:O7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="false" showRowColHeaders="1">
       <selection activeCell="A5" sqref="A5:O5"/>
@@ -562,23 +577,23 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:15">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
-      <c r="J2" s="1"/>
-      <c r="K2" s="1"/>
-      <c r="L2" s="1"/>
-      <c r="M2" s="1"/>
-      <c r="N2" s="1"/>
-      <c r="O2" s="1"/>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
+      <c r="J2" s="3"/>
+      <c r="K2" s="3"/>
+      <c r="L2" s="3"/>
+      <c r="M2" s="3"/>
+      <c r="N2" s="3"/>
+      <c r="O2" s="3"/>
     </row>
     <row r="3" spans="1:15">
       <c r="A3" s="3" t="s">
@@ -664,29 +679,103 @@
       </c>
     </row>
     <row r="6" spans="1:15">
-      <c r="A6" s="5" t="s">
+      <c r="A6" s="5">
+        <v>1</v>
+      </c>
+      <c r="B6" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="B6" s="5"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
-      <c r="G6" s="5"/>
-      <c r="H6" s="5"/>
-      <c r="I6" s="5"/>
-      <c r="J6" s="5"/>
-      <c r="K6" s="5"/>
-      <c r="L6" s="5"/>
-      <c r="M6" s="5"/>
-      <c r="N6" s="5"/>
-      <c r="O6" s="5"/>
+      <c r="C6" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="H6" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="I6" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="J6" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="K6" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="L6" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="M6" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="N6" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="O6" s="5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15">
+      <c r="A7" s="5">
+        <v>2</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="G7" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="H7" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="I7" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="J7" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="K7" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="L7" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="M7" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="N7" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="O7" s="5" t="s">
+        <v>32</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells>
     <mergeCell ref="A2:O2"/>
     <mergeCell ref="A3:O3"/>
-    <mergeCell ref="A6:O6"/>
   </mergeCells>
   <printOptions gridLines="false" gridLinesSet="true"/>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0.3" footer="0.3"/>
@@ -699,10 +788,10 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:O7"/>
+  <dimension ref="A1:O6"/>
   <sheetViews>
     <sheetView tabSelected="0" workbookViewId="0" showGridLines="false" showRowColHeaders="1">
-      <selection activeCell="A5" sqref="A5:L7"/>
+      <selection activeCell="A5" sqref="A5:L6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -721,20 +810,20 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:15">
-      <c r="A2" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
-      <c r="J2" s="1"/>
-      <c r="K2" s="1"/>
-      <c r="L2" s="1"/>
+      <c r="A2" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
+      <c r="J2" s="3"/>
+      <c r="K2" s="3"/>
+      <c r="L2" s="3"/>
       <c r="M2" s="1"/>
       <c r="N2" s="1"/>
       <c r="O2" s="1"/>
@@ -792,19 +881,19 @@
         <v>8</v>
       </c>
       <c r="G5" s="6" t="s">
-        <v>19</v>
+        <v>34</v>
       </c>
       <c r="H5" s="6" t="s">
-        <v>20</v>
+        <v>35</v>
       </c>
       <c r="I5" s="6" t="s">
-        <v>21</v>
+        <v>36</v>
       </c>
       <c r="J5" s="6" t="s">
-        <v>22</v>
+        <v>37</v>
       </c>
       <c r="K5" s="6" t="s">
-        <v>23</v>
+        <v>38</v>
       </c>
       <c r="L5" s="6" t="s">
         <v>16</v>
@@ -814,79 +903,41 @@
       <c r="O5" s="2"/>
     </row>
     <row r="6" spans="1:15">
-      <c r="A6" s="7">
+      <c r="A6" s="5">
         <v>1</v>
       </c>
-      <c r="B6" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="D6" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="E6" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="F6" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="G6" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="H6" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="I6" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="J6" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="K6" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="L6" s="7" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15">
-      <c r="A7" s="7">
-        <v>2</v>
-      </c>
-      <c r="B7" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="C7" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="D7" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="E7" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="F7" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="G7" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="H7" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="I7" s="7" t="s">
+      <c r="B6" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="J7" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="K7" s="7" t="s">
+      <c r="E6" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="L7" s="7" t="s">
+      <c r="F6" s="5" t="s">
         <v>41</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="H6" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="I6" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="J6" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="K6" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="L6" s="5" t="s">
+        <v>47</v>
       </c>
     </row>
   </sheetData>

</xml_diff>